<commit_message>
Ajout de format 1 2 et 3 de cnss, ajout de format cnamgs format1
</commit_message>
<xml_diff>
--- a/backend/public/DTS_CNSS_FORMAT2.xlsx
+++ b/backend/public/DTS_CNSS_FORMAT2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\joel\sega\backend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1F9746-30FE-448C-832C-70E8DF37A8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23C84E6-A533-493C-B10C-CC9FC76752EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>Matricule employeur</t>
   </si>
@@ -283,13 +283,16 @@
     <t>MASSE SALARIALE PLAFONNEE CNAMGS</t>
   </si>
   <si>
-    <t>[dts.msalcnamgs1;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[dts.msalcnamgs2;ope=tbs:num]</t>
-  </si>
-  <si>
-    <t>[dts.msalcnamgs3;ope=tbs:num]</t>
+    <t>[dts.msalcnam1;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[dts.msalcnam2;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[dts.msalcnam3;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[dts.msalcnamtotal;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +428,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -787,8 +798,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -798,135 +807,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -937,10 +817,141 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1498,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1671,12 +1682,12 @@
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1699,10 +1710,10 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="83"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
       <c r="E11" s="6" t="s">
@@ -1721,20 +1732,20 @@
       <c r="J11" s="1"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="63" t="s">
+      <c r="M11" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="84"/>
-      <c r="O11" s="84"/>
-      <c r="P11" s="85"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="91"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1743,20 +1754,20 @@
       <c r="J12" s="1"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="86" t="s">
+      <c r="M12" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="88"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="94"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1765,10 +1776,10 @@
       <c r="J13" s="1"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="74"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="80"/>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
@@ -1783,10 +1794,10 @@
       <c r="J14" s="1"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="77"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="83"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -1809,10 +1820,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="77"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="83"/>
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
@@ -1827,10 +1838,10 @@
       <c r="J16" s="1"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="77"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="83"/>
     </row>
     <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
@@ -1855,10 +1866,10 @@
       <c r="J17" s="1"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="80"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="86"/>
     </row>
     <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
@@ -1881,12 +1892,12 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="68"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1895,12 +1906,12 @@
       <c r="J19" s="1"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="63" t="s">
+      <c r="M19" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
-      <c r="P19" s="65"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
     </row>
     <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
@@ -1921,29 +1932,29 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="66" t="s">
+      <c r="M20" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="N20" s="67"/>
-      <c r="O20" s="67"/>
-      <c r="P20" s="68"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
     </row>
     <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="49" t="s">
+      <c r="C21" s="76"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="2"/>
       <c r="M21" s="16"/>
       <c r="N21" s="2"/>
@@ -1976,20 +1987,20 @@
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52" t="s">
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="61"/>
       <c r="L23" s="2"/>
       <c r="M23" s="19"/>
       <c r="N23" s="20"/>
@@ -2021,25 +2032,25 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="58" t="s">
+      <c r="G25" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="59"/>
-      <c r="I25" s="46" t="s">
+      <c r="H25" s="63"/>
+      <c r="I25" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="47"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="46" t="s">
+      <c r="J25" s="51"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="47"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="93" t="s">
+      <c r="M25" s="51"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="94"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52"/>
     </row>
     <row r="26" spans="1:17" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
@@ -2084,13 +2095,13 @@
       <c r="N26" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="O26" s="90" t="s">
+      <c r="O26" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="P26" s="91" t="s">
+      <c r="P26" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="Q26" s="92" t="s">
+      <c r="Q26" s="47" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2098,10 +2109,10 @@
       <c r="A27" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="44" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="32" t="s">
@@ -2110,7 +2121,7 @@
       <c r="E27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="45" t="s">
+      <c r="F27" s="43" t="s">
         <v>76</v>
       </c>
       <c r="G27" s="32" t="s">
@@ -2178,12 +2189,12 @@
       <c r="D29" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="43"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="41"/>
       <c r="I29" s="34" t="s">
         <v>63</v>
       </c>
@@ -2215,12 +2226,12 @@
       <c r="D30" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="43"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="41"/>
       <c r="I30" s="34" t="s">
         <v>82</v>
       </c>
@@ -2235,32 +2246,32 @@
         <v>84</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="Q30" s="36"/>
     </row>
     <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="37" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="Q31" s="38"/>
+      <c r="Q31" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>